<commit_message>
tz: chi: fixed some issues on forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_4_urine_filtration.xlsx
+++ b/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_4_urine_filtration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Tanzania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D9C876-FF1B-4EEE-A954-4116C9BEF0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E24DB2-6519-4BEE-BCC8-B88B8FD62FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="470">
   <si>
     <t>type</t>
   </si>
@@ -1321,24 +1321,9 @@
     <t>round( 10 * ${u_sh_egg} div ${u_urine_vol} )</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>u_end_note</t>
-  </si>
-  <si>
     <t>u_sch_man</t>
   </si>
   <si>
-    <t>u_urine_conserve</t>
-  </si>
-  <si>
-    <t>${u_urine_conserve} = 'Oui'</t>
-  </si>
-  <si>
-    <t>${u_urine_conserve} = 'Non'</t>
-  </si>
-  <si>
     <t>label::English</t>
   </si>
   <si>
@@ -1351,9 +1336,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>Was the child's urine preserved?</t>
-  </si>
-  <si>
     <t>Urine volume: Record the milliliters (ml) of urine collected from the person</t>
   </si>
   <si>
@@ -1366,9 +1348,6 @@
     <t>Number of eggs (S. Mansoni) per 10 ml</t>
   </si>
   <si>
-    <t>The child's urine was not preserved. You cannot save its results.</t>
-  </si>
-  <si>
     <t>Additional Notes</t>
   </si>
   <si>
@@ -1450,15 +1429,6 @@
     <t>Urine results</t>
   </si>
   <si>
-    <t>(2023 Nov) - 4. SCH/STH - Urine Filtration V1.2</t>
-  </si>
-  <si>
-    <t>tz_sch_sth_impact_202311_4_urine_filtration_v1_2</t>
-  </si>
-  <si>
-    <t>u_1_2</t>
-  </si>
-  <si>
     <t>not(selected(${C3}, ${u_code_id}))</t>
   </si>
   <si>
@@ -1466,6 +1436,15 @@
   </si>
   <si>
     <t>join(' ', ${u_code_id})</t>
+  </si>
+  <si>
+    <t>u_1_3</t>
+  </si>
+  <si>
+    <t>(2023 Nov) - 4. SCH/STH - Urine Filtration V1.3</t>
+  </si>
+  <si>
+    <t>tz_sch_sth_impact_202311_4_urine_filtration_v1_3</t>
   </si>
 </sst>
 </file>
@@ -2086,13 +2065,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2120,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>2</v>
@@ -2132,7 +2111,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>4</v>
@@ -2161,17 +2140,17 @@
         <v>9</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
@@ -2189,7 +2168,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="27"/>
@@ -2208,10 +2187,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="27"/>
@@ -2233,7 +2212,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="27"/>
@@ -2252,10 +2231,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="D6" s="29"/>
       <c r="E6" s="27"/>
@@ -2271,10 +2250,10 @@
     </row>
     <row r="7" spans="1:13" s="33" customFormat="1" ht="31.5">
       <c r="A7" s="27" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -2283,7 +2262,7 @@
       <c r="G7" s="29"/>
       <c r="H7" s="27"/>
       <c r="I7" s="27" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
@@ -2291,13 +2270,13 @@
     </row>
     <row r="8" spans="1:13" s="21" customFormat="1">
       <c r="A8" s="49" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="49"/>
@@ -2311,13 +2290,13 @@
     </row>
     <row r="9" spans="1:13" s="21" customFormat="1">
       <c r="A9" s="36" t="s">
+        <v>445</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>448</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>452</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>455</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>459</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="51"/>
@@ -2325,7 +2304,7 @@
       <c r="G9" s="37"/>
       <c r="H9" s="36"/>
       <c r="I9" s="36" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
@@ -2333,13 +2312,13 @@
     </row>
     <row r="10" spans="1:13" s="21" customFormat="1" ht="63">
       <c r="A10" s="36" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="51"/>
@@ -2347,7 +2326,7 @@
       <c r="G10" s="37"/>
       <c r="H10" s="36"/>
       <c r="I10" s="36" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
@@ -2358,18 +2337,18 @@
         <v>14</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="36"/>
       <c r="F11" s="27" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
@@ -2379,20 +2358,24 @@
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:13" s="39" customFormat="1">
+    <row r="12" spans="1:13" s="39" customFormat="1" ht="31.5">
       <c r="A12" s="28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>431</v>
+        <v>16</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="30"/>
+      <c r="F12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>18</v>
+      </c>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
       <c r="J12" s="27" t="s">
@@ -2401,184 +2384,162 @@
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
     </row>
-    <row r="13" spans="1:13" s="39" customFormat="1" ht="31.5">
+    <row r="13" spans="1:13" s="21" customFormat="1">
       <c r="A13" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>16</v>
+        <v>424</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D13" s="30"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="28" t="s">
-        <v>432</v>
-      </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="27" t="s">
+      <c r="E13" s="40"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-    </row>
-    <row r="14" spans="1:13" s="21" customFormat="1" ht="31.5">
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+    </row>
+    <row r="14" spans="1:13" s="21" customFormat="1">
       <c r="A14" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="40"/>
       <c r="F14" s="28"/>
       <c r="G14" s="41"/>
-      <c r="H14" s="28" t="s">
-        <v>432</v>
-      </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="28" t="s">
-        <v>10</v>
-      </c>
+      <c r="H14" s="28"/>
+      <c r="I14" s="40" t="s">
+        <v>427</v>
+      </c>
+      <c r="J14" s="28"/>
       <c r="K14" s="40"/>
       <c r="L14" s="40"/>
-    </row>
-    <row r="15" spans="1:13" s="21" customFormat="1" ht="31.5">
+      <c r="M14" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="21" customFormat="1">
       <c r="A15" s="28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>441</v>
+        <v>456</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="40"/>
       <c r="F15" s="28"/>
       <c r="G15" s="41"/>
-      <c r="H15" s="28" t="s">
-        <v>432</v>
-      </c>
-      <c r="I15" s="40" t="s">
-        <v>427</v>
-      </c>
-      <c r="J15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="K15" s="40"/>
       <c r="L15" s="40"/>
-      <c r="M15" s="21" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="16" spans="1:13" s="21" customFormat="1" ht="31.5">
       <c r="A16" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>430</v>
+        <v>457</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="40"/>
       <c r="F16" s="28"/>
       <c r="G16" s="41"/>
-      <c r="H16" s="28" t="s">
-        <v>432</v>
-      </c>
-      <c r="I16" s="40"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="40" t="s">
+        <v>458</v>
+      </c>
       <c r="J16" s="28" t="s">
         <v>10</v>
       </c>
       <c r="K16" s="40"/>
       <c r="L16" s="40"/>
     </row>
-    <row r="17" spans="1:12" s="21" customFormat="1" ht="31.5">
-      <c r="A17" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>464</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="28" t="s">
-        <v>432</v>
-      </c>
-      <c r="I17" s="40" t="s">
-        <v>465</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-    </row>
-    <row r="18" spans="1:12" s="38" customFormat="1" ht="31.5">
-      <c r="A18" s="36" t="s">
-        <v>428</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>429</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>443</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="28" t="s">
-        <v>433</v>
-      </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="53" t="s">
-        <v>462</v>
-      </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
+    <row r="17" spans="1:12">
+      <c r="A17" s="53" t="s">
+        <v>455</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+    </row>
+    <row r="18" spans="1:12" s="21" customFormat="1">
+      <c r="A18" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>437</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+    </row>
+    <row r="19" spans="1:12" s="21" customFormat="1">
+      <c r="A19" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
     </row>
     <row r="20" spans="1:12" s="21" customFormat="1">
       <c r="A20" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>444</v>
-      </c>
-      <c r="D20" s="30"/>
+        <v>22</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="40"/>
       <c r="F20" s="28"/>
       <c r="G20" s="41"/>
@@ -2588,55 +2549,19 @@
       <c r="K20" s="40"/>
       <c r="L20" s="40"/>
     </row>
-    <row r="21" spans="1:12" s="21" customFormat="1">
-      <c r="A21" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>21</v>
-      </c>
+    <row r="21" spans="1:12">
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="43"/>
       <c r="D21" s="44"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="41"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="44"/>
       <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="28"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-    </row>
-    <row r="22" spans="1:12" s="21" customFormat="1">
-      <c r="A22" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="42"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2668,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>25</v>
@@ -9652,13 +9577,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="21" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>